<commit_message>
More unit test fix when there is columns missings
</commit_message>
<xml_diff>
--- a/ExcelReader.Test/Files/simple.xlsx
+++ b/ExcelReader.Test/Files/simple.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MX05711629\KOF\code\ExcelReader\ExcelReader.Test\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA35E9E9-18A5-422C-9B82-9D28AF5374F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740FD6D2-968A-462D-806B-F9400477B1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,9 +26,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>Foo</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Missing</t>
   </si>
 </sst>
 </file>
@@ -214,7 +239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -250,4 +275,69 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C451FB04-4B12-4F8A-8ECE-15B7EFD16913}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>123</v>
+      </c>
+      <c r="D4" s="3">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More reader excel testing for big files
</commit_message>
<xml_diff>
--- a/ExcelReader.Test/Files/simple.xlsx
+++ b/ExcelReader.Test/Files/simple.xlsx
@@ -8,16 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MX05711629\KOF\code\ExcelReader\ExcelReader.Test\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740FD6D2-968A-462D-806B-F9400477B1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E57A9B8-5F8E-483A-A6F5-9635AE799FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -26,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="17">
   <si>
     <t>Hello</t>
   </si>
@@ -53,6 +69,30 @@
   </si>
   <si>
     <t>Missing</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Employee Date</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Jhon</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Samiel</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Tax</t>
   </si>
 </sst>
 </file>
@@ -101,20 +141,25 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -125,6 +170,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8D6ECA2F-D398-4BEE-A4FE-503148667B34}" name="Tabla1" displayName="Tabla1" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5" xr:uid="{8D6ECA2F-D398-4BEE-A4FE-503148667B34}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B41AD866-B703-48B9-882E-B898841BBD2B}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{5D09C081-03A0-4F37-94C9-FED0A080C242}" name="Employee Date" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{C909D51A-5703-4A15-9147-4DE3C0670774}" name="Salary"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -281,8 +338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C451FB04-4B12-4F8A-8ECE-15B7EFD16913}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -340,4 +397,578 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836E8C23-DF20-4CFC-9E52-1EEE3AF0BA4C}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>123</v>
+      </c>
+      <c r="D3" s="3">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC1E4D8-5AC7-48D2-ACD3-2B412C559662}">
+  <dimension ref="A1:AF3"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" s="3">
+        <v>12</v>
+      </c>
+      <c r="U1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="3">
+        <v>12</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="3">
+        <v>12</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF1" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3">
+        <v>123</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3">
+        <v>123</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3">
+        <v>123</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="3">
+        <v>123</v>
+      </c>
+      <c r="U2" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="3">
+        <v>123</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>123</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>123</v>
+      </c>
+      <c r="D3" s="3">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>123</v>
+      </c>
+      <c r="H3" s="3">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="3">
+        <v>123</v>
+      </c>
+      <c r="L3" s="3">
+        <v>12</v>
+      </c>
+      <c r="M3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="3">
+        <v>123</v>
+      </c>
+      <c r="P3" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="3">
+        <v>123</v>
+      </c>
+      <c r="T3" s="3">
+        <v>12</v>
+      </c>
+      <c r="U3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" s="3">
+        <v>123</v>
+      </c>
+      <c r="X3" s="3">
+        <v>12</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>123</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>12</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>123</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2757FB-7CED-458D-AEF8-B1E6E6D8E0F7}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>30846</v>
+      </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23759</v>
+      </c>
+      <c r="C3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>36750</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <v>34680</v>
+      </c>
+      <c r="C5">
+        <v>12044</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E85D0FB-033C-41B5-B3E1-5D1684FFE41C}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>30846</v>
+      </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23759</v>
+      </c>
+      <c r="C3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>36750</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <v>34680</v>
+      </c>
+      <c r="C5">
+        <v>12044</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F4B06E2-6E36-4005-A0B4-DF0F6A8DFCD4}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2">
+        <v>30846</v>
+      </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+      <c r="D2">
+        <f>C2*1.15</f>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23759</v>
+      </c>
+      <c r="C3">
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D4" si="0">C3*1.15</f>
+        <v>165.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>36750</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2">
+        <v>34680</v>
+      </c>
+      <c r="C5">
+        <v>12044</v>
+      </c>
+      <c r="D5" s="6">
+        <f>C5*1.15</f>
+        <v>13850.599999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>